<commit_message>
data exploration and results
</commit_message>
<xml_diff>
--- a/taban_Collection_Data.xlsx
+++ b/taban_Collection_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\School\Class\2025-2 Fall\ENT6707\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeige\Documents\School\ENR_PhD_Courses\6707_EntTech\GitRepo\zei_sem_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED823AA-14ED-4A3F-B94B-61F7A05EA5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0F8C7D-10AB-4CAB-8CD1-60AFDBCDFD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31110" yWindow="660" windowWidth="20805" windowHeight="14355" xr2:uid="{073B1799-5507-4E30-ABBC-AE747C6DE9F0}"/>
+    <workbookView xWindow="-3785" yWindow="-10015" windowWidth="13715" windowHeight="8740" activeTab="1" xr2:uid="{073B1799-5507-4E30-ABBC-AE747C6DE9F0}"/>
   </bookViews>
   <sheets>
     <sheet name="count_data" sheetId="1" r:id="rId1"/>
@@ -37,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="28">
   <si>
     <t>sample</t>
   </si>
   <si>
-    <t>GDD</t>
-  </si>
-  <si>
     <t>Jackson</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>Integer; the number of the sampling period over which the collection takes place. A unique number is given to each collection date.</t>
   </si>
   <si>
-    <t>Double; sum of Growing Degree Days (Base: 50F) over the two weeks since the previous collection event</t>
-  </si>
-  <si>
     <t>site</t>
   </si>
   <si>
@@ -91,6 +85,42 @@
   </si>
   <si>
     <t>count</t>
+  </si>
+  <si>
+    <t>rep</t>
+  </si>
+  <si>
+    <t>AvgTemp</t>
+  </si>
+  <si>
+    <t>AvgCDD</t>
+  </si>
+  <si>
+    <t>AvgGDD</t>
+  </si>
+  <si>
+    <t>cmCDD</t>
+  </si>
+  <si>
+    <t>cmGDD</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Double; average cooling degree days at the given site over the previous 2 weeks</t>
+  </si>
+  <si>
+    <t>Double; average growing degree days at the given site over the previous 2 weeks</t>
+  </si>
+  <si>
+    <t>Double; average air temperature (Celsius) at the given site over the previous 2 weeks</t>
+  </si>
+  <si>
+    <t>Double; sum of Growing Degree Days over the previous two weeks</t>
+  </si>
+  <si>
+    <t>Double; sum of Cooling Degree Days over the previous two weeks</t>
   </si>
 </sst>
 </file>
@@ -134,10 +164,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,46 +503,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F763FC16-37D7-447F-816D-31211A6696CB}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
         <v>45121</v>
@@ -519,19 +562,33 @@
       <c r="E2">
         <v>85</v>
       </c>
-      <c r="F2">
-        <v>313.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="3">
+        <v>23.428571428571427</v>
+      </c>
+      <c r="G2" s="3">
+        <v>9.1142857142857139</v>
+      </c>
+      <c r="H2" s="3">
+        <v>24.114285714285717</v>
+      </c>
+      <c r="I2">
+        <f>G2*14</f>
+        <v>127.6</v>
+      </c>
+      <c r="J2">
+        <f>H2*14</f>
+        <v>337.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1">
         <v>45135</v>
@@ -539,19 +596,33 @@
       <c r="E3">
         <v>56</v>
       </c>
-      <c r="F3">
-        <v>330.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="3">
+        <v>23.06428571428571</v>
+      </c>
+      <c r="G3" s="3">
+        <v>8.4571428571428573</v>
+      </c>
+      <c r="H3" s="3">
+        <v>23.457142857142856</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I61" si="0">G3*14</f>
+        <v>118.4</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J61" si="1">H3*14</f>
+        <v>328.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1">
         <v>45149</v>
@@ -559,19 +630,33 @@
       <c r="E4">
         <v>16</v>
       </c>
-      <c r="F4">
-        <v>313.39999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="3">
+        <v>22.385714285714283</v>
+      </c>
+      <c r="G4" s="3">
+        <v>7.2428571428571429</v>
+      </c>
+      <c r="H4" s="3">
+        <v>22.242857142857137</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>101.4</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>311.39999999999992</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1">
         <v>45163</v>
@@ -579,19 +664,33 @@
       <c r="E5">
         <v>8</v>
       </c>
-      <c r="F5">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="3">
+        <v>22.728571428571428</v>
+      </c>
+      <c r="G5" s="3">
+        <v>7.8785714285714272</v>
+      </c>
+      <c r="H5" s="3">
+        <v>22.857142857142861</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>110.29999999999998</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>320.00000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1">
         <v>45177</v>
@@ -599,19 +698,33 @@
       <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6">
-        <v>290.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="3">
+        <v>21.485714285714291</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5.8642857142857148</v>
+      </c>
+      <c r="H6" s="3">
+        <v>20.607142857142858</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>82.100000000000009</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>288.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
         <v>45191</v>
@@ -619,19 +732,33 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="3">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.77857142857142847</v>
+      </c>
+      <c r="H7" s="3">
+        <v>13.264285714285714</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>10.899999999999999</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>185.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1">
         <v>45205</v>
@@ -639,19 +766,33 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
-        <v>163.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="3">
+        <v>18.271428571428572</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.6785714285714286</v>
+      </c>
+      <c r="H8" s="3">
+        <v>14.835714285714287</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>207.70000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1">
         <v>45219</v>
@@ -659,19 +800,33 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
-        <v>66.900000000000006</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="3">
+        <v>11.450000000000001</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3.2071428571428577</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>44.900000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1">
         <v>45233</v>
@@ -679,19 +834,33 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
-        <v>47.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="3">
+        <v>10.1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>4.3071428571428578</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>60.300000000000011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1">
         <v>45408</v>
@@ -699,19 +868,33 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11">
-        <v>143.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="3">
+        <v>14.185714285714285</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1.0285714285714287</v>
+      </c>
+      <c r="H11" s="3">
+        <v>8.6142857142857139</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>14.400000000000002</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>120.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1">
         <v>45422</v>
@@ -719,19 +902,33 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12">
-        <v>133.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="3">
+        <v>19.314285714285713</v>
+      </c>
+      <c r="G12" s="3">
+        <v>2.4428571428571426</v>
+      </c>
+      <c r="H12" s="3">
+        <v>16.735714285714284</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>34.199999999999996</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>234.29999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1">
         <v>45436</v>
@@ -739,19 +936,33 @@
       <c r="E13">
         <v>2</v>
       </c>
-      <c r="F13">
-        <v>202.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="3">
+        <v>19.05</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2.8142857142857141</v>
+      </c>
+      <c r="H13" s="3">
+        <v>16.264285714285712</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>39.4</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>227.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1">
         <v>45450</v>
@@ -759,19 +970,33 @@
       <c r="E14">
         <v>3</v>
       </c>
-      <c r="F14">
-        <v>245.4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="3">
+        <v>19.457142857142859</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3.4499999999999997</v>
+      </c>
+      <c r="H14" s="3">
+        <v>16.971428571428572</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>48.3</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>237.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1">
         <v>45464</v>
@@ -779,19 +1004,33 @@
       <c r="E15">
         <v>17</v>
       </c>
-      <c r="F15">
-        <v>282.89999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="3">
+        <v>21.571428571428573</v>
+      </c>
+      <c r="G15" s="3">
+        <v>6.5428571428571427</v>
+      </c>
+      <c r="H15" s="3">
+        <v>20.75714285714286</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>91.6</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>290.60000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1">
         <v>45478</v>
@@ -799,19 +1038,33 @@
       <c r="E16">
         <v>31</v>
       </c>
-      <c r="F16">
-        <v>352.9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="3">
+        <v>23.857142857142858</v>
+      </c>
+      <c r="G16" s="3">
+        <v>9.9785714285714295</v>
+      </c>
+      <c r="H16" s="3">
+        <v>24.892857142857142</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>139.70000000000002</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>348.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1">
         <v>45121</v>
@@ -819,19 +1072,33 @@
       <c r="E17">
         <v>65</v>
       </c>
-      <c r="F17">
-        <v>313.3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="3">
+        <v>23.428571428571427</v>
+      </c>
+      <c r="G17" s="3">
+        <v>9.1142857142857139</v>
+      </c>
+      <c r="H17" s="3">
+        <v>24.114285714285717</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>127.6</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>337.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1">
         <v>45135</v>
@@ -839,19 +1106,33 @@
       <c r="E18">
         <v>159</v>
       </c>
-      <c r="F18">
-        <v>330.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="3">
+        <v>23.06428571428571</v>
+      </c>
+      <c r="G18" s="3">
+        <v>8.4571428571428573</v>
+      </c>
+      <c r="H18" s="3">
+        <v>23.457142857142856</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>118.4</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>328.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="1">
         <v>45149</v>
@@ -859,19 +1140,33 @@
       <c r="E19">
         <v>25</v>
       </c>
-      <c r="F19">
-        <v>313.39999999999998</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="3">
+        <v>22.385714285714283</v>
+      </c>
+      <c r="G19" s="3">
+        <v>7.2428571428571429</v>
+      </c>
+      <c r="H19" s="3">
+        <v>22.242857142857137</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>101.4</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>311.39999999999992</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1">
         <v>45163</v>
@@ -879,19 +1174,33 @@
       <c r="E20">
         <v>15</v>
       </c>
-      <c r="F20">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="3">
+        <v>22.728571428571428</v>
+      </c>
+      <c r="G20" s="3">
+        <v>7.8785714285714272</v>
+      </c>
+      <c r="H20" s="3">
+        <v>22.857142857142861</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>110.29999999999998</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>320.00000000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21" s="1">
         <v>45177</v>
@@ -899,19 +1208,33 @@
       <c r="E21">
         <v>6</v>
       </c>
-      <c r="F21">
-        <v>290.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="3">
+        <v>21.485714285714291</v>
+      </c>
+      <c r="G21" s="3">
+        <v>5.8642857142857148</v>
+      </c>
+      <c r="H21" s="3">
+        <v>20.607142857142858</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>82.100000000000009</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>288.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1">
         <v>45191</v>
@@ -919,19 +1242,33 @@
       <c r="E22">
         <v>1</v>
       </c>
-      <c r="F22">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="3">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.77857142857142847</v>
+      </c>
+      <c r="H22" s="3">
+        <v>13.264285714285714</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>10.899999999999999</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>185.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="1">
         <v>45205</v>
@@ -939,19 +1276,33 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23">
-        <v>163.4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="3">
+        <v>18.271428571428572</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.6785714285714286</v>
+      </c>
+      <c r="H23" s="3">
+        <v>14.835714285714287</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>207.70000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1">
         <v>45219</v>
@@ -959,19 +1310,33 @@
       <c r="E24">
         <v>0</v>
       </c>
-      <c r="F24">
-        <v>66.900000000000006</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="3">
+        <v>11.450000000000001</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>3.2071428571428577</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>44.900000000000006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" s="1">
         <v>45233</v>
@@ -979,19 +1344,33 @@
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25">
-        <v>47.3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="3">
+        <v>10.1</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>4.3071428571428578</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>60.300000000000011</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1">
         <v>45408</v>
@@ -999,19 +1378,33 @@
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26">
-        <v>143.6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="3">
+        <v>14.185714285714285</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1.0285714285714287</v>
+      </c>
+      <c r="H26" s="3">
+        <v>8.6142857142857139</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>14.400000000000002</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>120.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1">
         <v>45422</v>
@@ -1019,19 +1412,33 @@
       <c r="E27">
         <v>1</v>
       </c>
-      <c r="F27">
-        <v>133.1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="3">
+        <v>19.314285714285713</v>
+      </c>
+      <c r="G27" s="3">
+        <v>2.4428571428571426</v>
+      </c>
+      <c r="H27" s="3">
+        <v>16.735714285714284</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>34.199999999999996</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>234.29999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" s="1">
         <v>45436</v>
@@ -1039,19 +1446,33 @@
       <c r="E28">
         <v>2</v>
       </c>
-      <c r="F28">
-        <v>202.7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="3">
+        <v>19.05</v>
+      </c>
+      <c r="G28" s="3">
+        <v>2.8142857142857141</v>
+      </c>
+      <c r="H28" s="3">
+        <v>16.264285714285712</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>39.4</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>227.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D29" s="1">
         <v>45450</v>
@@ -1059,19 +1480,33 @@
       <c r="E29">
         <v>6</v>
       </c>
-      <c r="F29">
-        <v>245.4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="3">
+        <v>19.457142857142859</v>
+      </c>
+      <c r="G29" s="3">
+        <v>3.4499999999999997</v>
+      </c>
+      <c r="H29" s="3">
+        <v>16.971428571428572</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>48.3</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>237.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30" s="1">
         <v>45464</v>
@@ -1079,19 +1514,33 @@
       <c r="E30">
         <v>25</v>
       </c>
-      <c r="F30">
-        <v>282.89999999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="3">
+        <v>21.571428571428573</v>
+      </c>
+      <c r="G30" s="3">
+        <v>6.5428571428571427</v>
+      </c>
+      <c r="H30" s="3">
+        <v>20.75714285714286</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>91.6</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>290.60000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D31" s="1">
         <v>45478</v>
@@ -1099,19 +1548,33 @@
       <c r="E31">
         <v>93</v>
       </c>
-      <c r="F31">
-        <v>352.9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="3">
+        <v>23.857142857142858</v>
+      </c>
+      <c r="G31" s="3">
+        <v>9.9785714285714295</v>
+      </c>
+      <c r="H31" s="3">
+        <v>24.892857142857142</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>139.70000000000002</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>348.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D32" s="1">
         <v>45121</v>
@@ -1119,19 +1582,33 @@
       <c r="E32">
         <v>3</v>
       </c>
-      <c r="F32">
-        <v>283.3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="3">
+        <v>22.519841269841269</v>
+      </c>
+      <c r="G32" s="3">
+        <v>7.4857142857142858</v>
+      </c>
+      <c r="H32" s="3">
+        <v>22.485714285714288</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>104.8</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>314.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33" s="1">
         <v>45135</v>
@@ -1139,19 +1616,33 @@
       <c r="E33">
         <v>11</v>
       </c>
-      <c r="F33">
-        <v>299.10000000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="3">
+        <v>22.107142857142861</v>
+      </c>
+      <c r="G33" s="3">
+        <v>6.7357142857142867</v>
+      </c>
+      <c r="H33" s="3">
+        <v>21.735714285714288</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>94.300000000000011</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>304.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D34" s="1">
         <v>45149</v>
@@ -1159,19 +1650,33 @@
       <c r="E34">
         <v>6</v>
       </c>
-      <c r="F34">
-        <v>286.10000000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="3">
+        <v>20.714285714285715</v>
+      </c>
+      <c r="G34" s="3">
+        <v>4.2357142857142858</v>
+      </c>
+      <c r="H34" s="3">
+        <v>19.235714285714284</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>59.3</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>269.29999999999995</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D35" s="1">
         <v>45163</v>
@@ -1179,19 +1684,33 @@
       <c r="E35">
         <v>3</v>
       </c>
-      <c r="F35">
-        <v>249.2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="3">
+        <v>20.559523809523807</v>
+      </c>
+      <c r="G35" s="3">
+        <v>4.2785714285714294</v>
+      </c>
+      <c r="H35" s="3">
+        <v>18.957142857142856</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>59.900000000000013</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="1"/>
+        <v>265.39999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D36" s="1">
         <v>45177</v>
@@ -1199,19 +1718,33 @@
       <c r="E36">
         <v>5</v>
       </c>
-      <c r="F36">
-        <v>282.8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="3">
+        <v>20.753968253968253</v>
+      </c>
+      <c r="G36" s="3">
+        <v>4.7857142857142865</v>
+      </c>
+      <c r="H36" s="3">
+        <v>19.321428571428573</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>67.000000000000014</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>270.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D37" s="1">
         <v>45191</v>
@@ -1219,19 +1752,33 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37">
-        <v>140.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="3">
+        <v>15.674603174603174</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3">
+        <v>10.185714285714285</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="1"/>
+        <v>142.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D38" s="1">
         <v>45205</v>
@@ -1239,19 +1786,33 @@
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38">
-        <v>143.19999999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="3">
+        <v>17.257936507936506</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0.40714285714285708</v>
+      </c>
+      <c r="H38" s="3">
+        <v>13.014285714285714</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>5.6999999999999993</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>182.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D39" s="1">
         <v>45219</v>
@@ -1259,19 +1820,33 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39">
-        <v>60.3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="3">
+        <v>9.988095238095239</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3">
+        <v>1.5928571428571427</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>22.299999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D40" s="1">
         <v>45233</v>
@@ -1279,19 +1854,33 @@
       <c r="E40">
         <v>0</v>
       </c>
-      <c r="F40">
-        <v>15.9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="3">
+        <v>9.5595238095238084</v>
+      </c>
+      <c r="G40" s="3">
+        <v>7.1428571428571435E-3</v>
+      </c>
+      <c r="H40" s="3">
+        <v>4.2357142857142858</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="1"/>
+        <v>59.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D41" s="1">
         <v>45408</v>
@@ -1299,19 +1888,33 @@
       <c r="E41">
         <v>0</v>
       </c>
-      <c r="F41">
-        <v>95.2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="3">
+        <v>11.531746031746033</v>
+      </c>
+      <c r="G41" s="3">
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="H41" s="3">
+        <v>5.3285714285714283</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="1"/>
+        <v>74.599999999999994</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D42" s="1">
         <v>45422</v>
@@ -1319,19 +1922,33 @@
       <c r="E42">
         <v>0</v>
       </c>
-      <c r="F42">
-        <v>111.6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="3">
+        <v>18.210317460317462</v>
+      </c>
+      <c r="G42" s="3">
+        <v>2.3642857142857139</v>
+      </c>
+      <c r="H42" s="3">
+        <v>14.728571428571428</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="0"/>
+        <v>33.099999999999994</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="1"/>
+        <v>206.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D43" s="1">
         <v>45436</v>
@@ -1339,19 +1956,33 @@
       <c r="E43">
         <v>0</v>
       </c>
-      <c r="F43">
-        <v>165.4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="3">
+        <v>18.638888888888889</v>
+      </c>
+      <c r="G43" s="3">
+        <v>2.75</v>
+      </c>
+      <c r="H43" s="3">
+        <v>15.542857142857143</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="0"/>
+        <v>38.5</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="1"/>
+        <v>217.6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D44" s="1">
         <v>45450</v>
@@ -1359,19 +1990,33 @@
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="F44">
-        <v>229.7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="3">
+        <v>18.388888888888886</v>
+      </c>
+      <c r="G44" s="3">
+        <v>2.4928571428571429</v>
+      </c>
+      <c r="H44" s="3">
+        <v>15.042857142857141</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>34.9</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="1"/>
+        <v>210.59999999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D45" s="1">
         <v>45464</v>
@@ -1379,19 +2024,33 @@
       <c r="E45">
         <v>0</v>
       </c>
-      <c r="F45">
-        <v>225.4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="3">
+        <v>21.043650793650791</v>
+      </c>
+      <c r="G45" s="3">
+        <v>6.2714285714285714</v>
+      </c>
+      <c r="H45" s="3">
+        <v>19.828571428571429</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="0"/>
+        <v>87.8</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="1"/>
+        <v>277.60000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D46" s="1">
         <v>45478</v>
@@ -1399,19 +2058,33 @@
       <c r="E46">
         <v>1</v>
       </c>
-      <c r="F46">
-        <v>327.9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="3">
+        <v>22.210317460317462</v>
+      </c>
+      <c r="G46" s="3">
+        <v>7.1714285714285717</v>
+      </c>
+      <c r="H46" s="3">
+        <v>21.942857142857143</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="0"/>
+        <v>100.4</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="1"/>
+        <v>307.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D47" s="1">
         <v>45121</v>
@@ -1419,19 +2092,33 @@
       <c r="E47">
         <v>5</v>
       </c>
-      <c r="F47">
-        <v>283.3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="3">
+        <v>22.519841269841269</v>
+      </c>
+      <c r="G47" s="3">
+        <v>7.4857142857142858</v>
+      </c>
+      <c r="H47" s="3">
+        <v>22.485714285714288</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="0"/>
+        <v>104.8</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="1"/>
+        <v>314.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D48" s="1">
         <v>45135</v>
@@ -1439,19 +2126,33 @@
       <c r="E48">
         <v>39</v>
       </c>
-      <c r="F48">
-        <v>299.10000000000002</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="3">
+        <v>22.107142857142861</v>
+      </c>
+      <c r="G48" s="3">
+        <v>6.7357142857142867</v>
+      </c>
+      <c r="H48" s="3">
+        <v>21.735714285714288</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="0"/>
+        <v>94.300000000000011</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="1"/>
+        <v>304.3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D49" s="1">
         <v>45149</v>
@@ -1459,19 +2160,33 @@
       <c r="E49">
         <v>7</v>
       </c>
-      <c r="F49">
-        <v>286.10000000000002</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="3">
+        <v>20.714285714285715</v>
+      </c>
+      <c r="G49" s="3">
+        <v>4.2357142857142858</v>
+      </c>
+      <c r="H49" s="3">
+        <v>19.235714285714284</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="0"/>
+        <v>59.3</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="1"/>
+        <v>269.29999999999995</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D50" s="1">
         <v>45163</v>
@@ -1479,19 +2194,33 @@
       <c r="E50">
         <v>13</v>
       </c>
-      <c r="F50">
-        <v>249.2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="3">
+        <v>20.559523809523807</v>
+      </c>
+      <c r="G50" s="3">
+        <v>4.2785714285714294</v>
+      </c>
+      <c r="H50" s="3">
+        <v>18.957142857142856</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="0"/>
+        <v>59.900000000000013</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="1"/>
+        <v>265.39999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D51" s="1">
         <v>45177</v>
@@ -1499,19 +2228,33 @@
       <c r="E51">
         <v>0</v>
       </c>
-      <c r="F51">
-        <v>282.8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="3">
+        <v>20.753968253968253</v>
+      </c>
+      <c r="G51" s="3">
+        <v>4.7857142857142865</v>
+      </c>
+      <c r="H51" s="3">
+        <v>19.321428571428573</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="0"/>
+        <v>67.000000000000014</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="1"/>
+        <v>270.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D52" s="1">
         <v>45191</v>
@@ -1519,19 +2262,33 @@
       <c r="E52">
         <v>0</v>
       </c>
-      <c r="F52">
-        <v>140.5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="3">
+        <v>15.674603174603174</v>
+      </c>
+      <c r="G52" s="3">
+        <v>0</v>
+      </c>
+      <c r="H52" s="3">
+        <v>10.185714285714285</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="1"/>
+        <v>142.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D53" s="1">
         <v>45205</v>
@@ -1539,19 +2296,33 @@
       <c r="E53">
         <v>0</v>
       </c>
-      <c r="F53">
-        <v>143.19999999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="3">
+        <v>17.257936507936506</v>
+      </c>
+      <c r="G53" s="3">
+        <v>0.40714285714285708</v>
+      </c>
+      <c r="H53" s="3">
+        <v>13.014285714285714</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="0"/>
+        <v>5.6999999999999993</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="1"/>
+        <v>182.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D54" s="1">
         <v>45219</v>
@@ -1559,19 +2330,33 @@
       <c r="E54">
         <v>0</v>
       </c>
-      <c r="F54">
-        <v>60.3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="3">
+        <v>9.988095238095239</v>
+      </c>
+      <c r="G54" s="3">
+        <v>0</v>
+      </c>
+      <c r="H54" s="3">
+        <v>1.5928571428571427</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="1"/>
+        <v>22.299999999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D55" s="1">
         <v>45233</v>
@@ -1579,19 +2364,33 @@
       <c r="E55">
         <v>0</v>
       </c>
-      <c r="F55">
-        <v>15.9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F55" s="3">
+        <v>9.5595238095238084</v>
+      </c>
+      <c r="G55" s="3">
+        <v>7.1428571428571435E-3</v>
+      </c>
+      <c r="H55" s="3">
+        <v>4.2357142857142858</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="1"/>
+        <v>59.3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D56" s="1">
         <v>45408</v>
@@ -1599,19 +2398,33 @@
       <c r="E56">
         <v>0</v>
       </c>
-      <c r="F56">
-        <v>95.2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="3">
+        <v>11.531746031746033</v>
+      </c>
+      <c r="G56" s="3">
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="H56" s="3">
+        <v>5.3285714285714283</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="1"/>
+        <v>74.599999999999994</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D57" s="1">
         <v>45422</v>
@@ -1619,19 +2432,33 @@
       <c r="E57">
         <v>0</v>
       </c>
-      <c r="F57">
-        <v>111.6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="3">
+        <v>18.210317460317462</v>
+      </c>
+      <c r="G57" s="3">
+        <v>2.3642857142857139</v>
+      </c>
+      <c r="H57" s="3">
+        <v>14.728571428571428</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="0"/>
+        <v>33.099999999999994</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="1"/>
+        <v>206.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D58" s="1">
         <v>45436</v>
@@ -1639,19 +2466,33 @@
       <c r="E58">
         <v>0</v>
       </c>
-      <c r="F58">
-        <v>165.4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F58" s="3">
+        <v>18.638888888888889</v>
+      </c>
+      <c r="G58" s="3">
+        <v>2.75</v>
+      </c>
+      <c r="H58" s="3">
+        <v>15.542857142857143</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="0"/>
+        <v>38.5</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="1"/>
+        <v>217.6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>13</v>
       </c>
       <c r="B59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D59" s="1">
         <v>45450</v>
@@ -1659,19 +2500,33 @@
       <c r="E59">
         <v>2</v>
       </c>
-      <c r="F59">
-        <v>229.7</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="3">
+        <v>18.388888888888886</v>
+      </c>
+      <c r="G59" s="3">
+        <v>2.4928571428571429</v>
+      </c>
+      <c r="H59" s="3">
+        <v>15.042857142857141</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="0"/>
+        <v>34.9</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="1"/>
+        <v>210.59999999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>14</v>
       </c>
       <c r="B60" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D60" s="1">
         <v>45464</v>
@@ -1679,19 +2534,33 @@
       <c r="E60">
         <v>5</v>
       </c>
-      <c r="F60">
-        <v>225.4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="3">
+        <v>21.043650793650791</v>
+      </c>
+      <c r="G60" s="3">
+        <v>6.2714285714285714</v>
+      </c>
+      <c r="H60" s="3">
+        <v>19.828571428571429</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="0"/>
+        <v>87.8</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="1"/>
+        <v>277.60000000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>15</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D61" s="1">
         <v>45478</v>
@@ -1699,8 +2568,22 @@
       <c r="E61">
         <v>7</v>
       </c>
-      <c r="F61">
-        <v>327.9</v>
+      <c r="F61" s="3">
+        <v>22.210317460317462</v>
+      </c>
+      <c r="G61" s="3">
+        <v>7.1714285714285717</v>
+      </c>
+      <c r="H61" s="3">
+        <v>21.942857142857143</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="0"/>
+        <v>100.4</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="1"/>
+        <v>307.2</v>
       </c>
     </row>
   </sheetData>
@@ -1710,71 +2593,103 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC1C8917-CE89-4EDB-A220-AE4353D8D614}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>